<commit_message>
- udpated test workbook with data inside - updated test cases that already relied on this workbook - added reader for the worksheet titles
</commit_message>
<xml_diff>
--- a/src/tests/test_data/genuine/empty.xlsx
+++ b/src/tests/test_data/genuine/empty.xlsx
@@ -4,20 +4,38 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="24795" windowHeight="12255"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="24795" windowHeight="12255" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1 - Text" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2 - Numbers" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3 - Formulas" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="2">
+  <si>
+    <t>This is cell A1 in Sheet 1</t>
+  </si>
+  <si>
+    <t>This is cell G5</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -43,14 +61,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -342,36 +363,304 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="G5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="D1:K30"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="4:11">
+      <c r="D1">
+        <v>1</v>
+      </c>
+      <c r="K1" s="1">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="2" spans="4:11">
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="K2" s="1">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="3" spans="4:11">
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="K3" s="1">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="4" spans="4:11">
+      <c r="D4">
+        <v>4</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="5" spans="4:11">
+      <c r="D5">
+        <v>5</v>
+      </c>
+      <c r="G5" t="s">
+        <v>1</v>
+      </c>
+      <c r="K5" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="6" spans="4:11">
+      <c r="D6">
+        <v>6</v>
+      </c>
+      <c r="K6" s="1">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="7" spans="4:11">
+      <c r="D7">
+        <v>7</v>
+      </c>
+      <c r="K7" s="1">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="4:11">
+      <c r="D8">
+        <v>8</v>
+      </c>
+      <c r="K8" s="1">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="9" spans="4:11">
+      <c r="D9">
+        <v>9</v>
+      </c>
+      <c r="K9" s="1">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="10" spans="4:11">
+      <c r="D10">
+        <v>10</v>
+      </c>
+      <c r="K10" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="11" spans="4:11">
+      <c r="D11">
+        <v>11</v>
+      </c>
+      <c r="K11" s="1">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="12" spans="4:11">
+      <c r="D12">
+        <v>12</v>
+      </c>
+      <c r="K12" s="1">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="13" spans="4:11">
+      <c r="D13">
+        <v>13</v>
+      </c>
+      <c r="K13" s="1">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="14" spans="4:11">
+      <c r="D14">
+        <v>14</v>
+      </c>
+      <c r="K14" s="1">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="4:11">
+      <c r="D15">
+        <v>15</v>
+      </c>
+      <c r="K15" s="1">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="16" spans="4:11">
+      <c r="D16">
+        <v>16</v>
+      </c>
+      <c r="K16" s="1">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="17" spans="4:11">
+      <c r="D17">
+        <v>17</v>
+      </c>
+      <c r="K17" s="1">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="18" spans="4:11">
+      <c r="D18">
+        <v>18</v>
+      </c>
+      <c r="K18" s="1">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="19" spans="4:11">
+      <c r="D19">
+        <v>19</v>
+      </c>
+      <c r="K19" s="1">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="20" spans="4:11">
+      <c r="D20">
+        <v>20</v>
+      </c>
+      <c r="K20" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="21" spans="4:11">
+      <c r="D21">
+        <v>21</v>
+      </c>
+      <c r="K21" s="1">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="22" spans="4:11">
+      <c r="D22">
+        <v>22</v>
+      </c>
+      <c r="K22" s="1">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="23" spans="4:11">
+      <c r="D23">
+        <v>23</v>
+      </c>
+      <c r="K23" s="1">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="24" spans="4:11">
+      <c r="D24">
+        <v>24</v>
+      </c>
+      <c r="K24" s="1">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="25" spans="4:11">
+      <c r="D25">
+        <v>25</v>
+      </c>
+      <c r="K25" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="26" spans="4:11">
+      <c r="D26">
+        <v>26</v>
+      </c>
+      <c r="K26" s="1">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="27" spans="4:11">
+      <c r="D27">
+        <v>27</v>
+      </c>
+      <c r="K27" s="1">
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="28" spans="4:11">
+      <c r="D28">
+        <v>28</v>
+      </c>
+      <c r="K28" s="1">
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="29" spans="4:11">
+      <c r="D29">
+        <v>29</v>
+      </c>
+      <c r="K29" s="1">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="30" spans="4:11">
+      <c r="D30">
+        <v>30</v>
+      </c>
+      <c r="K30" s="1">
+        <v>0.3</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="2" spans="4:4">
+      <c r="D2">
+        <f>'Sheet2 - Numbers'!D5</f>
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>